<commit_message>
modif exam et plot theme
</commit_message>
<xml_diff>
--- a/Exam/ExoTD/2020-11-05/grades.xlsx
+++ b/Exam/ExoTD/2020-11-05/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colin/Travail/Enseignements/R/Exam/ExoTD/2020-11-05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A77D064-FAE6-AC41-A9ED-4EC38D8A0A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F0D093-6F9C-E844-A152-EE96CE02A05E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B5AD9CED-9E63-D545-AB8E-7FD645B63A4E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>kiourtzidou_aikaterini</t>
   </si>
@@ -86,9 +86,6 @@
     <t>anik_ahmed</t>
   </si>
   <si>
-    <t>Grade2</t>
-  </si>
-  <si>
     <t>Grade1</t>
   </si>
   <si>
@@ -117,6 +114,12 @@
   </si>
   <si>
     <t>fit and plot</t>
+  </si>
+  <si>
+    <t>Grade3</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
 </sst>
 </file>
@@ -495,121 +498,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C49868-6EDB-3B43-A0D2-5FCA112DBBCB}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" customWidth="1"/>
-    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" customWidth="1"/>
+    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2">
-        <f>SUM(D2:Y2)</f>
+        <f>SUM(E2:Y2)</f>
         <v>21</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1">
-        <v>3</v>
-      </c>
-      <c r="J2" s="1">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1">
-        <v>2</v>
-      </c>
-      <c r="M2" s="1">
-        <v>1</v>
-      </c>
-      <c r="N2" s="1">
-        <v>3</v>
-      </c>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="2">
+        <f>SUM(E2:Z2)</f>
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -617,44 +628,48 @@
         <v>10</v>
       </c>
       <c r="C3" s="2">
-        <f>MIN(SUM(D3:N3),20)</f>
+        <f>MIN(SUM(E3:N3),20)</f>
         <v>3.5</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="D3" s="2">
+        <f>MAX(B3,MIN(SUM(E3:O3),20))</f>
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>0.5</v>
       </c>
-      <c r="J3" s="3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3">
-        <v>0</v>
-      </c>
-      <c r="M3" s="3">
-        <v>0</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -662,44 +677,48 @@
         <v>19</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C15" si="0">MIN(SUM(D4:N4),20)</f>
+        <f t="shared" ref="C4:C15" si="0">MIN(SUM(E4:N4),20)</f>
+        <v>17</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="C4:D15" si="1">MAX(B4,MIN(SUM(E4:O4),20))</f>
         <v>19</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>3</v>
       </c>
       <c r="J4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -708,13 +727,47 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>11.5</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>2.5</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -723,13 +776,47 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>13.25</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="1"/>
+        <v>13.25</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1.5</v>
+      </c>
+      <c r="H6">
+        <v>0.5</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>2.75</v>
+      </c>
+      <c r="K6">
+        <v>1.5</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -738,13 +825,47 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>11.75</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="1"/>
+        <v>12.75</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1.5</v>
+      </c>
+      <c r="G7">
+        <v>2.5</v>
+      </c>
+      <c r="H7">
+        <v>0.5</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>2.75</v>
+      </c>
+      <c r="K7">
+        <v>0.5</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -753,43 +874,47 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8">
         <v>2</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -798,13 +923,47 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>2.5</v>
+      </c>
+      <c r="J9">
+        <v>2.5</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -813,13 +972,47 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>16.5</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
+        <v>16.5</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>3.5</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -828,13 +1021,47 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.5</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>2.5</v>
+      </c>
+      <c r="K11">
+        <v>1.5</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -843,13 +1070,47 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>0.5</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0.5</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>2.5</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0.5</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,13 +1119,47 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>15.5</v>
+      </c>
+      <c r="D13" s="2">
+        <f>MAX(B13,MIN(SUM(E13:O13),20))</f>
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>2.5</v>
+      </c>
+      <c r="K13">
+        <v>1.5</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1.5</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -873,13 +1168,47 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>12.5</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>1.5</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -888,14 +1217,48 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1.5</v>
+      </c>
+      <c r="H15">
+        <v>0.5</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>2.5</v>
+      </c>
+      <c r="K15">
+        <v>1.5</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1.5</v>
+      </c>
+      <c r="N15">
+        <v>0.5</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L15">
     <sortCondition ref="A2:A15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>